<commit_message>
Primka di modifiche a variazione spedizione
</commit_message>
<xml_diff>
--- a/WEB_Auto/DocumentiXTelai/TXT/GNV_TEST-NON-USARE_30-07-2021_T0000000.XLSX
+++ b/WEB_Auto/DocumentiXTelai/TXT/GNV_TEST-NON-USARE_30-07-2021_T0000000.XLSX
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <x:si>
     <x:t>Astrea Claim Solutions S.r.l.</x:t>
   </x:si>
@@ -94,28 +94,25 @@
     <x:t>Note</x:t>
   </x:si>
   <x:si>
-    <x:t>TR01</x:t>
+    <x:t>TEST01</x:t>
   </x:si>
   <x:si>
     <x:t>1241-ROLLING GOODS</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">103-LUCIANU LOGISTICA </x:t>
+    <x:t>100-LO CICERO ANTONINO</x:t>
   </x:si>
   <x:si>
     <x:t>GOOD</x:t>
   </x:si>
   <x:si>
-    <x:t>TR02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>104-MAGLIONE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TR03</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">101-LOGISTICA MEDITERRANEA </x:t>
+    <x:t>TEST02</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">102-LOGISTICA NIEDDU </x:t>
+  </x:si>
+  <x:si>
+    <x:t>TEST03</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -564,7 +561,7 @@
     <x:col min="1" max="1" width="25.820625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="21.040625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="12.260625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="28.850625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="24.790625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="8.380625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="8.050625" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="13.110625" style="0" customWidth="1"/>
@@ -718,7 +715,7 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C12" s="8">
-        <x:v>44407.4258101852</x:v>
+        <x:v>44407.4915625</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>28</x:v>
@@ -738,7 +735,7 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C13" s="8">
-        <x:v>44407.4259027778</x:v>
+        <x:v>44407.4917013889</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>31</x:v>
@@ -758,10 +755,10 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C14" s="8">
-        <x:v>44407.4260069444</x:v>
+        <x:v>44407.4923726852</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
         <x:v>29</x:v>

</xml_diff>